<commit_message>
Register the first four weaknesses.
</commit_message>
<xml_diff>
--- a/Actividad 01 - Identificación Hallazgos BD.xlsx
+++ b/Actividad 01 - Identificación Hallazgos BD.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/69367ade8eb4dc32/UTN/2025/I/ISW-1012/1.Clases/02/Actividades/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crisa\OneDrive\Documents\UTN\l Cuatrimestre\Auditoría de Sistemas\Actividades\Actividad 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="242" documentId="8_{64D213E2-CCAF-46E4-BB7B-2BC9B7E08BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DD77797-F7EB-486B-BEAD-7F5797572793}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9296A959-D89A-4A2A-BEC0-791B0230B3FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52635" yWindow="2580" windowWidth="23895" windowHeight="15345" activeTab="2" xr2:uid="{124CE4B9-C2B7-444E-982F-07D767DED2D4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{124CE4B9-C2B7-444E-982F-07D767DED2D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Instrucciones" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
   <si>
     <t>#</t>
   </si>
@@ -104,6 +104,27 @@
   </si>
   <si>
     <t>Entregar nombre de archivo de la siguiente manera: Actividad06_&lt;Numero grupo&gt;.xlsx</t>
+  </si>
+  <si>
+    <t>Integridad de Entidad - Llave Primaria</t>
+  </si>
+  <si>
+    <t>Integridad de Entidad - Llave Única</t>
+  </si>
+  <si>
+    <t>Integridad de Dominio</t>
+  </si>
+  <si>
+    <t>En la base de datos "ISW1012" en el esquema "actividad01" en la tabla "cliente" específicamente en la columna "id" no define un mecanismo automático para la generación de los identificadores únicos, lo que podría generar conflictos al insertar nuevos registros si no se gestionan adecuadamente los valores.</t>
+  </si>
+  <si>
+    <t>En la base de datos "ISW1012" en el esquema "actividad01" en la tabla "cliente" específicamente en la columna "correo" no se identifica la definición de una restricción de unicidad, lo que permite la posibilidad de registros duplicados en los correos electrónicos de los clientes, afectando la integridad y consistencia de los datos.</t>
+  </si>
+  <si>
+    <t>En la base de datos "ISW1012" en el esquema "actividad01" en la tabla "cliente" específicamente en la columna "correo" no existe la validación de su formato y longitud, permitiendo el ingreso de valores diferentes a correos electrónicos y omitiendo la limitación estándar de 320 caracteres, lo que podría afectar la integridad de los datos y restringir el registro de ciertos usuarios.</t>
+  </si>
+  <si>
+    <t>En la base de datos "ISW1012" en el esquema "actividad01" en la tabla "cliente" específicamente en la columna "fecha_creacion" permite el ingreso de valores sin restricciones de rango,  lo que posibilita el registro de fechas futuras o extremadamente antiguas.</t>
   </si>
 </sst>
 </file>
@@ -141,7 +162,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -191,11 +212,67 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -236,17 +313,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -256,6 +325,37 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -271,10 +371,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -577,16 +673,16 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.5703125" customWidth="1"/>
-    <col min="2" max="2" width="116.140625" customWidth="1"/>
+    <col min="1" max="1" width="2.5546875" customWidth="1"/>
+    <col min="2" max="2" width="116.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -597,7 +693,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -606,7 +702,7 @@
       </c>
       <c r="C2" s="11"/>
     </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -617,7 +713,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -628,23 +724,23 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6"/>
       <c r="B5" s="7"/>
       <c r="C5" s="13"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C6">
         <f>SUM(C2:C5)</f>
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="19" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="7" t="s">
         <v>20</v>
       </c>
@@ -656,182 +752,201 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C29F3FA1-80F2-4D2C-83A9-CB5A3A9C490C}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" customWidth="1"/>
-    <col min="2" max="2" width="66.5703125" customWidth="1"/>
-    <col min="3" max="3" width="31.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" customWidth="1"/>
+    <col min="2" max="2" width="66.5546875" customWidth="1"/>
+    <col min="3" max="3" width="31.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
+    <row r="2" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" s="18">
         <v>1</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="15"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="14">
+      <c r="B2" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="28"/>
+    </row>
+    <row r="3" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3" s="18">
         <v>2</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="14"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="14">
+      <c r="B3" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="29"/>
+    </row>
+    <row r="4" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A4" s="18">
         <v>3</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="14"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="14">
+      <c r="B4" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="25"/>
+    </row>
+    <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="18">
         <v>4</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="14"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="14">
+      <c r="B5" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="25"/>
+      <c r="F5" s="30"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="18">
         <v>5</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="14"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="14">
+      <c r="B6" s="19"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="25"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="18">
         <v>6</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="14"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="14">
+      <c r="B7" s="19"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="25"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="18">
         <v>7</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="14"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="14">
+      <c r="B8" s="19"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="25"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="18">
         <v>8</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="14"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="14">
+      <c r="B9" s="19"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="25"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="18">
         <v>9</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="14"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
+      <c r="B10" s="19"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="25"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="18">
         <v>10</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="20"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="14">
+      <c r="B11" s="20"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="16"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="18">
         <v>11</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="14"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="14">
+      <c r="B12" s="19"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="25"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="18">
         <v>12</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="14"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="14">
+      <c r="B13" s="19"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="25"/>
+      <c r="F13" s="24"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="18">
         <v>13</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="14"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="14">
+      <c r="B14" s="19"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="25"/>
+      <c r="F14" s="24"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="18">
         <v>14</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="14"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="14">
+      <c r="B15" s="19"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="25"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="18">
         <v>15</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="14"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="14">
+      <c r="B16" s="19"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="25"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="18">
         <v>16</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="14"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="14">
+      <c r="B17" s="19"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="25"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="18">
         <v>17</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="14"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="14">
+      <c r="B18" s="19"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="25"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="18">
         <v>18</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="14"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="25"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -842,191 +957,191 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA170A17-B9E1-4EAC-B91E-27670B2B139F}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="101.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="2" max="2" width="101.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="21"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="17"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="3"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="5"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="5"/>
     </row>
-    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="7"/>
     </row>
-    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="21" t="s">
+    <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="21"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="17"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="5"/>
     </row>
-    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="7"/>
     </row>
-    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="21" t="s">
+    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="21"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="17"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B16" s="5"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="5"/>
     </row>
-    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B18" s="7"/>
     </row>
-    <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="21" t="s">
+    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="21"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="17"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B21" s="3"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B22" s="5"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B23" s="5"/>
     </row>
-    <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B24" s="7"/>
     </row>
-    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="21" t="s">
+    <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="21"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="17"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B26" s="3"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B27" s="3"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B28" s="5"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B29" s="5"/>
     </row>
-    <row r="30" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="10" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Register the weaknesses from 5 to 7.
</commit_message>
<xml_diff>
--- a/Actividad 01 - Identificación Hallazgos BD.xlsx
+++ b/Actividad 01 - Identificación Hallazgos BD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crisa\OneDrive\Documents\UTN\l Cuatrimestre\Auditoría de Sistemas\Actividades\Actividad 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9296A959-D89A-4A2A-BEC0-791B0230B3FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1F18C3-C4D8-4527-8B5B-A879C6DAFF2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{124CE4B9-C2B7-444E-982F-07D767DED2D4}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
   <si>
     <t>#</t>
   </si>
@@ -125,6 +125,18 @@
   </si>
   <si>
     <t>En la base de datos "ISW1012" en el esquema "actividad01" en la tabla "cliente" específicamente en la columna "fecha_creacion" permite el ingreso de valores sin restricciones de rango,  lo que posibilita el registro de fechas futuras o extremadamente antiguas.</t>
+  </si>
+  <si>
+    <t>En la base de datos "ISW1012" en el esquema "actividad01" en la tabla "producto" no se identifica la definición de restricción de clave primaria (primary key) sobre la columna "id".</t>
+  </si>
+  <si>
+    <t>En la base de datos "ISW1012", dentro del esquema "actividad01", en la tabla "producto" no se identifica la definición de una restricción de unicidad sobre la columna "codigo", esto permite la existencia de productos con códigos duplicados.</t>
+  </si>
+  <si>
+    <t>Integridad de Atributo</t>
+  </si>
+  <si>
+    <t>En la base de datos "ISW1012", dentro del esquema "actividad01", en la tabla "producto" específicamente en la columna "nombre" se permite el ingreso de valores nulos y en blanco, permitiendo la perdida de un dato esencial para la identificación y descripción de los productos.</t>
   </si>
 </sst>
 </file>
@@ -272,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -322,16 +334,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -341,7 +347,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -355,7 +360,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -752,10 +765,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C29F3FA1-80F2-4D2C-83A9-CB5A3A9C490C}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -766,7 +779,7 @@
     <col min="4" max="4" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -780,169 +793,178 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A2" s="18">
+    <row r="2" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" s="17">
         <v>1</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="28"/>
-    </row>
-    <row r="3" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A3" s="18">
+      <c r="D2" s="25"/>
+    </row>
+    <row r="3" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3" s="17">
         <v>2</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="29"/>
-    </row>
-    <row r="4" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A4" s="18">
+      <c r="D3" s="26"/>
+    </row>
+    <row r="4" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A4" s="17">
         <v>3</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="25"/>
-    </row>
-    <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="18">
+      <c r="D4" s="22"/>
+    </row>
+    <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="17">
         <v>4</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="25"/>
-      <c r="F5" s="30"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="18">
+      <c r="D5" s="22"/>
+    </row>
+    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="17">
         <v>5</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="25"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="18">
+      <c r="B6" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="22"/>
+    </row>
+    <row r="7" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="17">
         <v>6</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="25"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="18">
+      <c r="B7" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="22"/>
+    </row>
+    <row r="8" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="17">
         <v>7</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="25"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="18">
+      <c r="B8" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="22"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="17">
         <v>8</v>
       </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="25"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="18">
+      <c r="B9" s="28"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="22"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="17">
         <v>9</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="25"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="18">
+      <c r="B10" s="28"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="22"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="17">
         <v>10</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="19"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="18"/>
       <c r="E11" s="16"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="18">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="17">
         <v>11</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="25"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="18">
+      <c r="B12" s="28"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="22"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="17">
         <v>12</v>
       </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="25"/>
-      <c r="F13" s="24"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="18">
+      <c r="B13" s="28"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="22"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="17">
         <v>13</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="25"/>
-      <c r="F14" s="24"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="18">
+      <c r="B14" s="28"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="22"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="17">
         <v>14</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="25"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="18">
+      <c r="B15" s="28"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="22"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="17">
         <v>15</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="25"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="22"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="18">
+      <c r="A17" s="17">
         <v>16</v>
       </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="25"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="22"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="18">
+      <c r="A18" s="17">
         <v>17</v>
       </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="25"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="22"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="18">
+      <c r="A19" s="17">
         <v>18</v>
       </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="25"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="22"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D22" s="16"/>
@@ -968,10 +990,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -1004,10 +1026,10 @@
       <c r="B6" s="7"/>
     </row>
     <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="17"/>
+      <c r="B7" s="27"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
@@ -1040,10 +1062,10 @@
       <c r="B12" s="7"/>
     </row>
     <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="17"/>
+      <c r="B13" s="27"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
@@ -1076,10 +1098,10 @@
       <c r="B18" s="7"/>
     </row>
     <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="17"/>
+      <c r="B19" s="27"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
@@ -1112,10 +1134,10 @@
       <c r="B24" s="7"/>
     </row>
     <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="17"/>
+      <c r="B25" s="27"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">

</xml_diff>

<commit_message>
Register the weaknesses from 7 to 15.
</commit_message>
<xml_diff>
--- a/Actividad 01 - Identificación Hallazgos BD.xlsx
+++ b/Actividad 01 - Identificación Hallazgos BD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crisa\OneDrive\Documents\UTN\l Cuatrimestre\Auditoría de Sistemas\Actividades\Actividad 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1F18C3-C4D8-4527-8B5B-A879C6DAFF2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33116BE-48A0-4124-A8AF-EFF0EC44CD8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{124CE4B9-C2B7-444E-982F-07D767DED2D4}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="44">
   <si>
     <t>#</t>
   </si>
@@ -136,7 +136,43 @@
     <t>Integridad de Atributo</t>
   </si>
   <si>
-    <t>En la base de datos "ISW1012", dentro del esquema "actividad01", en la tabla "producto" específicamente en la columna "nombre" se permite el ingreso de valores nulos y en blanco, permitiendo la perdida de un dato esencial para la identificación y descripción de los productos.</t>
+    <t>En la base de datos "ISW1012", dentro del esquema "actividad01", en la tabla "producto" específicamente la columna "nombre" se permite el ingreso de valores nulos y en blanco, permitiendo la perdida de un dato esencial para la identificación y descripción de los productos.</t>
+  </si>
+  <si>
+    <t>Integridad de Dominio*</t>
+  </si>
+  <si>
+    <t>En la base de datos "ISW1012", dentro del esquema "actividad01", en la tabla "producto" específicamente en la columna "precio" no se establece una restricción que valide que el valor pertenezca a un conjunto válido de datos, ya que permite ingresar valores negativos.</t>
+  </si>
+  <si>
+    <t>En la base de datos "ISW1012", dentro del esquema "actividad01", en la tabla "producto", específicamente en la columna "descripcion" se permiten valores extremadamente largos (hasta 10 000 caracteres), lo que es excesivo para los posibles valores del campo, ocupando más espacio en disco.</t>
+  </si>
+  <si>
+    <t>En la base de datos "ISW1012", dentro del esquema "actividad01",  en la columna "descripcion" de la tabla "producto" no cuenta con una restricción para impedir el ingreso de valores en blanco o nulos, lo que podría generar inconsistencias en la base de datos.</t>
+  </si>
+  <si>
+    <t>En la base de datos "ISW1012", dentro del esquema "actividad01", en la tabla "pedido", específicamente la columna "monto_total" no una restricción que impida el ingreso de valores negativos o iguales a cero, lo que podría generar inconsistencias ya que reflejaría montos de compra inválidos.</t>
+  </si>
+  <si>
+    <t>Integridad de Usuario o Negocio</t>
+  </si>
+  <si>
+    <t>En la base de datos "ISW1012", dentro del esquema "actividad01", en la columna "monto_total" de la tabla "pedido" no cuenta con una validación que asegure su coherencia con la suma de los subtotales de los detalles del pedido, lo que llevar a inconsistencias en la información financiera.</t>
+  </si>
+  <si>
+    <t>En la base de datos "ISW1012", dentro del esquema "actividad01", en la tabla "pedido", específicamente en la columna "fecha" no existe una restricción que impida la inserción de fechas futuras o extremadamente antiguas, lo cuál es problemático.</t>
+  </si>
+  <si>
+    <t>Integridad referencial</t>
+  </si>
+  <si>
+    <t>En la base de datos "ISW1012", dentro del esquema "actividad01", en la tabla "pedido_detalle" específicamente la columna "id_producto" no cuenta con una restricción de clave foranea que garantice  la relación con la tabla "producto".</t>
+  </si>
+  <si>
+    <t>Integridad de usuario o negocio</t>
+  </si>
+  <si>
+    <t>En la base de datos "ISW1012", dentro del esquema "actividad01", en la tabla "pedido_detalle", específicamente en la columna "subtotal", no existe un proceso que garantice que su valor sea coherente con la multiplicación del precio unitario del producto por la cantidad solicitada. Lo que podría generar inconsistencias en los datos financieros.</t>
   </si>
 </sst>
 </file>
@@ -174,7 +210,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -280,11 +316,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -360,13 +407,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -767,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C29F3FA1-80F2-4D2C-83A9-CB5A3A9C490C}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -821,7 +871,7 @@
       <c r="A4" s="17">
         <v>3</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="27" t="s">
         <v>26</v>
       </c>
       <c r="C4" s="20" t="s">
@@ -833,7 +883,7 @@
       <c r="A5" s="17">
         <v>4</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="27" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="20" t="s">
@@ -845,7 +895,7 @@
       <c r="A6" s="17">
         <v>5</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="27" t="s">
         <v>28</v>
       </c>
       <c r="C6" s="20" t="s">
@@ -857,7 +907,7 @@
       <c r="A7" s="17">
         <v>6</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="27" t="s">
         <v>29</v>
       </c>
       <c r="C7" s="20" t="s">
@@ -869,7 +919,7 @@
       <c r="A8" s="17">
         <v>7</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="27" t="s">
         <v>31</v>
       </c>
       <c r="C8" s="20" t="s">
@@ -877,76 +927,108 @@
       </c>
       <c r="D8" s="22"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="17">
         <v>8</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="20"/>
+      <c r="B9" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>23</v>
+      </c>
       <c r="D9" s="22"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="17">
         <v>9</v>
       </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="20"/>
+      <c r="B10" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>30</v>
+      </c>
       <c r="D10" s="22"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="17">
         <v>10</v>
       </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="21"/>
+      <c r="B11" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>32</v>
+      </c>
       <c r="D11" s="18"/>
       <c r="E11" s="16"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="17">
         <v>11</v>
       </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="20"/>
+      <c r="B12" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>32</v>
+      </c>
       <c r="D12" s="22"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="17">
         <v>12</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="20"/>
+      <c r="B13" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>37</v>
+      </c>
       <c r="D13" s="22"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="17">
         <v>13</v>
       </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="20"/>
+      <c r="B14" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>23</v>
+      </c>
       <c r="D14" s="22"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="17">
         <v>14</v>
       </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="20"/>
+      <c r="B15" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>40</v>
+      </c>
       <c r="D15" s="22"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="17">
         <v>15</v>
       </c>
-      <c r="B16" s="28"/>
-      <c r="C16" s="20"/>
+      <c r="B16" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="D16" s="22"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="17">
         <v>16</v>
       </c>
-      <c r="B17" s="28"/>
+      <c r="B17" s="27"/>
       <c r="C17" s="20"/>
       <c r="D17" s="22"/>
     </row>
@@ -954,7 +1036,7 @@
       <c r="A18" s="17">
         <v>17</v>
       </c>
-      <c r="B18" s="28"/>
+      <c r="B18" s="27"/>
       <c r="C18" s="20"/>
       <c r="D18" s="22"/>
     </row>
@@ -962,7 +1044,7 @@
       <c r="A19" s="17">
         <v>18</v>
       </c>
-      <c r="B19" s="28"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="20"/>
       <c r="D19" s="22"/>
     </row>
@@ -990,10 +1072,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="27"/>
+      <c r="B1" s="29"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -1026,10 +1108,10 @@
       <c r="B6" s="7"/>
     </row>
     <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="27"/>
+      <c r="B7" s="29"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
@@ -1062,10 +1144,10 @@
       <c r="B12" s="7"/>
     </row>
     <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="27"/>
+      <c r="B13" s="29"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
@@ -1098,10 +1180,10 @@
       <c r="B18" s="7"/>
     </row>
     <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="27"/>
+      <c r="B19" s="29"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
@@ -1134,10 +1216,10 @@
       <c r="B24" s="7"/>
     </row>
     <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="27" t="s">
+      <c r="A25" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="27"/>
+      <c r="B25" s="29"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">

</xml_diff>

<commit_message>
Add the record for two findings.
</commit_message>
<xml_diff>
--- a/Actividad 01 - Identificación Hallazgos BD.xlsx
+++ b/Actividad 01 - Identificación Hallazgos BD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crisa\OneDrive\Documents\UTN\l Cuatrimestre\Auditoría de Sistemas\Actividades\Actividad 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33116BE-48A0-4124-A8AF-EFF0EC44CD8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C22078-EE6D-4717-8D5C-B257A0D0022F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{124CE4B9-C2B7-444E-982F-07D767DED2D4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{124CE4B9-C2B7-444E-982F-07D767DED2D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Instrucciones" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="54">
   <si>
     <t>#</t>
   </si>
@@ -173,6 +173,36 @@
   </si>
   <si>
     <t>En la base de datos "ISW1012", dentro del esquema "actividad01", en la tabla "pedido_detalle", específicamente en la columna "subtotal", no existe un proceso que garantice que su valor sea coherente con la multiplicación del precio unitario del producto por la cantidad solicitada. Lo que podría generar inconsistencias en los datos financieros.</t>
+  </si>
+  <si>
+    <t>Posibilidad de que no se pueda identificar un producto de forma única.</t>
+  </si>
+  <si>
+    <t>Regla de integridad de Entidad - Llave Primaria</t>
+  </si>
+  <si>
+    <t>En la base de datos "ISW1012", dentro del esquema "actividad01", la tabla "producto" no cuenta con la definición de una restricción de clave primaria (PRIMARY KEY).</t>
+  </si>
+  <si>
+    <t>Definir una restricción de clave primaria para la columna "id" de la tabla "producto" del esquema "actividad01" de la base de datos "ISW1012", asegurando que cada producto tenga un identificador único.</t>
+  </si>
+  <si>
+    <t>Deficiencia en el proceso de diseño de base de datos, donde no se definió explícitamente una clave primaria en la tabla "producto" dentro del esquema "actividad01".</t>
+  </si>
+  <si>
+    <t>En la base de datos "ISW1012", dentro del esquema "actividad01", la tabla "pedido_detalle" no posee una restricción de clave foránea (FOREIGN KEY) para la columna "id_producto".</t>
+  </si>
+  <si>
+    <t>Deficiencia en el proceso de diseño de base de datos, donde no se definió explícitamente una clave foránea en la tabla "pedido_detalle" que referencie a la tabla "producto".</t>
+  </si>
+  <si>
+    <t>Posibilidad de registrar productos en "detalle_pedidos" con una referencia inválida de algún registro de la tabla "producto".</t>
+  </si>
+  <si>
+    <t>Regla de Integridad Referencial - Llave foránea.</t>
+  </si>
+  <si>
+    <t>Definir una restricción de clave foránea para la columna "id_producto" de la tabla "pedido_detall"e, referenciando la clave primaria de la tabla "producto" dentro del esquema "actividad01" en la base de datos "ISW1012".</t>
   </si>
 </sst>
 </file>
@@ -331,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -382,9 +412,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -394,30 +421,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -736,7 +759,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -817,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C29F3FA1-80F2-4D2C-83A9-CB5A3A9C490C}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView showGridLines="0" topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -847,206 +870,210 @@
       <c r="A2" s="17">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="25"/>
+      <c r="D2" s="26"/>
     </row>
     <row r="3" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="17">
         <v>2</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="26"/>
+      <c r="D3" s="20"/>
     </row>
     <row r="4" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="17">
         <v>3</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="22"/>
+      <c r="D4" s="20"/>
     </row>
     <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="17">
         <v>4</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="22"/>
+      <c r="D5" s="20"/>
     </row>
     <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="17">
         <v>5</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="22"/>
+      <c r="D6" s="20" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="17">
         <v>6</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="22"/>
+      <c r="D7" s="20"/>
     </row>
     <row r="8" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="17">
         <v>7</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="22"/>
+      <c r="D8" s="20"/>
     </row>
     <row r="9" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="17">
         <v>8</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="22"/>
+      <c r="D9" s="20"/>
     </row>
     <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="17">
         <v>9</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="22"/>
+      <c r="D10" s="20"/>
     </row>
     <row r="11" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="17">
         <v>10</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="18"/>
+      <c r="D11" s="19"/>
       <c r="E11" s="16"/>
     </row>
     <row r="12" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="17">
         <v>11</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="22"/>
+      <c r="D12" s="20"/>
     </row>
     <row r="13" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="17">
         <v>12</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="22"/>
+      <c r="D13" s="20"/>
     </row>
     <row r="14" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="17">
         <v>13</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="22"/>
+      <c r="D14" s="20"/>
     </row>
     <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="17">
         <v>14</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="22"/>
+      <c r="D15" s="20" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="17">
         <v>15</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="22"/>
+      <c r="D16" s="20"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="17">
         <v>16</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="22"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="20"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="17">
         <v>17</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="22"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="20"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="17">
         <v>18</v>
       </c>
-      <c r="B19" s="27"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="22"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="20"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D22" s="16"/>
@@ -1061,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA170A17-B9E1-4EAC-B91E-27670B2B139F}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1072,46 +1099,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="29"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1" s="27"/>
+    </row>
+    <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5"/>
-    </row>
-    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="7"/>
+      <c r="B6" s="7" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="29"/>
+      <c r="B7" s="27"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
@@ -1144,10 +1181,10 @@
       <c r="B12" s="7"/>
     </row>
     <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="29"/>
+      <c r="B13" s="27"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
@@ -1180,46 +1217,56 @@
       <c r="B18" s="7"/>
     </row>
     <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="29"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B19" s="27"/>
+    </row>
+    <row r="20" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="3"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B21" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="5"/>
+      <c r="B22" s="5" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="5"/>
-    </row>
-    <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="7"/>
+      <c r="B24" s="7" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="29" t="s">
+      <c r="A25" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="29"/>
+      <c r="B25" s="27"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">

</xml_diff>

<commit_message>
Add one finding and update some errors in weaknesses.
</commit_message>
<xml_diff>
--- a/Actividad 01 - Identificación Hallazgos BD.xlsx
+++ b/Actividad 01 - Identificación Hallazgos BD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crisa\OneDrive\Documents\UTN\l Cuatrimestre\Auditoría de Sistemas\Actividades\Actividad 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C22078-EE6D-4717-8D5C-B257A0D0022F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FBCC67-9163-4700-8436-ACA6E08FC71D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{124CE4B9-C2B7-444E-982F-07D767DED2D4}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="64">
   <si>
     <t>#</t>
   </si>
@@ -121,9 +121,6 @@
     <t>En la base de datos "ISW1012" en el esquema "actividad01" en la tabla "cliente" específicamente en la columna "correo" no se identifica la definición de una restricción de unicidad, lo que permite la posibilidad de registros duplicados en los correos electrónicos de los clientes, afectando la integridad y consistencia de los datos.</t>
   </si>
   <si>
-    <t>En la base de datos "ISW1012" en el esquema "actividad01" en la tabla "cliente" específicamente en la columna "correo" no existe la validación de su formato y longitud, permitiendo el ingreso de valores diferentes a correos electrónicos y omitiendo la limitación estándar de 320 caracteres, lo que podría afectar la integridad de los datos y restringir el registro de ciertos usuarios.</t>
-  </si>
-  <si>
     <t>En la base de datos "ISW1012" en el esquema "actividad01" en la tabla "cliente" específicamente en la columna "fecha_creacion" permite el ingreso de valores sin restricciones de rango,  lo que posibilita el registro de fechas futuras o extremadamente antiguas.</t>
   </si>
   <si>
@@ -202,7 +199,40 @@
     <t>Regla de Integridad Referencial - Llave foránea.</t>
   </si>
   <si>
-    <t>Definir una restricción de clave foránea para la columna "id_producto" de la tabla "pedido_detall"e, referenciando la clave primaria de la tabla "producto" dentro del esquema "actividad01" en la base de datos "ISW1012".</t>
+    <t>Definir una restricción de clave foránea para la columna "id_producto" de la tabla "pedido_detalle", referenciando la clave primaria de la tabla "producto" dentro del esquema "actividad01" en la base de datos "ISW1012".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hallazgo 01 - </t>
+  </si>
+  <si>
+    <t>En la base de datos "ISW1012" en el esquema "actividad01"  en la columna "correo" de la tabla "cliente" existe un límite de longitud de 100, omitiendo la limitación estándar de 320 caracteres, lo que puede restringir el registro de posibles usuarios.</t>
+  </si>
+  <si>
+    <t>En la base de datos "ISW1012" en el esquema "actividad01" en la tabla "cliente" específicamente en la columna "correo" no existe la validación de su formato, permitiendo el ingreso de valores que no corresponden a direcciones de correo electrónico válidas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En la base de datos "ISW1012", dentro del esquema "actividad01", en la tabla "pedido_detalle", la columna "cantidad" no cuenta con una validación que verifique la disponibilidad de stock en la tabla "producto" antes de registrar un pedido. </t>
+  </si>
+  <si>
+    <t>En la base de datos "ISW1012", dentro del esquema "actividad01", la columna "correo" de la tabla "cliente" tiene un límite de longitud de 100 caracteres, lo que restringe la entrada de direcciones de correo electrónico más largas.</t>
+  </si>
+  <si>
+    <t>Deficiencia en el proceso de diseño de la base de datos, donde no se consideró el estándar internacional que permite hasta 320 caracteres en direcciones de correo electrónico.</t>
+  </si>
+  <si>
+    <t>Posibilidad de que algunos clientes no puedan registrarse si sus direcciones de correo electrónico superan el límite de 100 caracteres.</t>
+  </si>
+  <si>
+    <t>Regla de Integridad de Dominio</t>
+  </si>
+  <si>
+    <t>Modificar la definición de la columna correo en la tabla cliente para que utilice el tipo de dato "VARCHAR(320)", permitiendo almacenar direcciones de correo electrónico con el máximo de caracteres definidos por los estándares internacionales.</t>
+  </si>
+  <si>
+    <t>Regla de Integridad de Atributo</t>
+  </si>
+  <si>
+    <t>Regla de Integridad de Usuario o Negocio</t>
   </si>
 </sst>
 </file>
@@ -240,7 +270,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -357,11 +387,59 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -441,6 +519,19 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -838,10 +929,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C29F3FA1-80F2-4D2C-83A9-CB5A3A9C490C}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -890,15 +981,15 @@
       </c>
       <c r="D3" s="20"/>
     </row>
-    <row r="4" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="17">
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="D4" s="20"/>
     </row>
@@ -907,48 +998,50 @@
         <v>4</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="20"/>
-    </row>
-    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D5" s="20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="17">
         <v>5</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="D6" s="20"/>
+    </row>
+    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="17">
         <v>6</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="20"/>
+        <v>21</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="17">
         <v>7</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D8" s="20"/>
     </row>
@@ -957,10 +1050,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D9" s="20"/>
     </row>
@@ -969,10 +1062,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D10" s="20"/>
     </row>
@@ -980,36 +1073,36 @@
       <c r="A11" s="17">
         <v>10</v>
       </c>
-      <c r="B11" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="16"/>
+      <c r="B11" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="20"/>
     </row>
     <row r="12" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="17">
         <v>11</v>
       </c>
-      <c r="B12" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="19" t="s">
+      <c r="B12" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="20"/>
+      <c r="C12" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="19"/>
+      <c r="E12" s="16"/>
     </row>
     <row r="13" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="17">
         <v>12</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D13" s="20"/>
     </row>
@@ -1017,54 +1110,62 @@
       <c r="A14" s="17">
         <v>13</v>
       </c>
-      <c r="B14" s="25" t="s">
-        <v>39</v>
+      <c r="B14" s="23" t="s">
+        <v>37</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="D14" s="20"/>
     </row>
-    <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="17">
         <v>14</v>
       </c>
-      <c r="B15" s="23" t="s">
-        <v>41</v>
+      <c r="B15" s="25" t="s">
+        <v>38</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="D15" s="20"/>
+    </row>
+    <row r="16" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="17">
         <v>15</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="20"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="17">
         <v>16</v>
       </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="19"/>
+      <c r="B17" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>41</v>
+      </c>
       <c r="D17" s="20"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A18" s="17">
         <v>17</v>
       </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="19"/>
+      <c r="B18" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>41</v>
+      </c>
       <c r="D18" s="20"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1075,9 +1176,9 @@
       <c r="C19" s="19"/>
       <c r="D19" s="20"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1086,10 +1187,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA170A17-B9E1-4EAC-B91E-27670B2B139F}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1098,205 +1199,232 @@
     <col min="2" max="2" width="101.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="27"/>
-    </row>
-    <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="B1" s="28"/>
+    </row>
+    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B2" s="31" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="C3" s="29"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" s="30" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+      <c r="C5" s="29"/>
+    </row>
+    <row r="6" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+      <c r="C6" s="29"/>
+    </row>
+    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="27"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" s="28"/>
+    </row>
+    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="29"/>
+    </row>
+    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="3"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B9" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="29"/>
+    </row>
+    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="5"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="29"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="5"/>
-    </row>
-    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="29"/>
+    </row>
+    <row r="12" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="7"/>
-    </row>
-    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="27"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B13" s="28"/>
+    </row>
+    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="3"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B14" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="29"/>
+    </row>
+    <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="3"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="29"/>
+    </row>
+    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="5"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B16" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="29"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="5"/>
-    </row>
-    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="7"/>
-    </row>
-    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="29"/>
+    </row>
+    <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="27"/>
-    </row>
-    <row r="20" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B19" s="28"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B20" s="3"/>
+      <c r="C20" s="29"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B21" s="30"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B22" s="5"/>
+      <c r="C22" s="29"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="32"/>
+    </row>
+    <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="27"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B25" s="28"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="3"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B26" s="31"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="3"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B27" s="30"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="5"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B28" s="30"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B29" s="5"/>
-    </row>
-    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B30" s="7"/>
+      <c r="B30" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>